<commit_message>
poblando la tabla alineacion y equipo v1
</commit_message>
<xml_diff>
--- a/poblarTorneoFutbol.xlsx
+++ b/poblarTorneoFutbol.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Materias\SSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731ED3C3-1B60-483C-A7F4-BE9CD355D25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02331ACF-399E-4147-87D9-1AA169E616D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Nombres" sheetId="1" r:id="rId1"/>
     <sheet name="Estadio" sheetId="4" r:id="rId2"/>
     <sheet name="Equipos" sheetId="3" r:id="rId3"/>
-    <sheet name="Apellidos" sheetId="2" r:id="rId4"/>
-    <sheet name="Tecnicos" sheetId="5" r:id="rId5"/>
+    <sheet name="Dirigentes" sheetId="6" r:id="rId4"/>
+    <sheet name="Apellidos" sheetId="2" r:id="rId5"/>
+    <sheet name="Tecnicos" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="720">
   <si>
     <t>Hugo</t>
   </si>
@@ -2545,8 +2546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C52DDD2-28BF-4C94-8ED5-EF6546E9B4DB}">
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D558" sqref="D558"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="B200" sqref="B200:B250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9268,7 +9269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE44EE9-E27F-40A6-848A-C6B51C889E69}">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -9442,6 +9443,586 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F6090D-08DD-4213-90E6-B42BF7439D3C}">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46:E47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B1" t="s">
+        <v>671</v>
+      </c>
+      <c r="C1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>548</v>
+      </c>
+      <c r="C3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C4" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>550</v>
+      </c>
+      <c r="C5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>551</v>
+      </c>
+      <c r="C6" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>552</v>
+      </c>
+      <c r="C7" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>553</v>
+      </c>
+      <c r="C8" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>554</v>
+      </c>
+      <c r="C9" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>555</v>
+      </c>
+      <c r="C10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>556</v>
+      </c>
+      <c r="C11" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>557</v>
+      </c>
+      <c r="C12" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>558</v>
+      </c>
+      <c r="C13" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>559</v>
+      </c>
+      <c r="C14" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>560</v>
+      </c>
+      <c r="C15" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>561</v>
+      </c>
+      <c r="C16" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>556</v>
+      </c>
+      <c r="C17" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>562</v>
+      </c>
+      <c r="C18" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C19" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>564</v>
+      </c>
+      <c r="C20" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>565</v>
+      </c>
+      <c r="C21" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>566</v>
+      </c>
+      <c r="C22" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>567</v>
+      </c>
+      <c r="C23" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>568</v>
+      </c>
+      <c r="C24" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>569</v>
+      </c>
+      <c r="C25" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>570</v>
+      </c>
+      <c r="C26" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>571</v>
+      </c>
+      <c r="C27" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>572</v>
+      </c>
+      <c r="C28" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>573</v>
+      </c>
+      <c r="C29" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>574</v>
+      </c>
+      <c r="C30" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>575</v>
+      </c>
+      <c r="C31" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>576</v>
+      </c>
+      <c r="C32" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>577</v>
+      </c>
+      <c r="C33" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
+        <v>578</v>
+      </c>
+      <c r="C34" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
+        <v>585</v>
+      </c>
+      <c r="C35" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="s">
+        <v>586</v>
+      </c>
+      <c r="C36" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>587</v>
+      </c>
+      <c r="C37" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>588</v>
+      </c>
+      <c r="C38" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" t="s">
+        <v>589</v>
+      </c>
+      <c r="C39" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
+        <v>590</v>
+      </c>
+      <c r="C40" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>591</v>
+      </c>
+      <c r="C41" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" t="s">
+        <v>592</v>
+      </c>
+      <c r="C42" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" t="s">
+        <v>593</v>
+      </c>
+      <c r="C43" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" t="s">
+        <v>594</v>
+      </c>
+      <c r="C44" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" t="s">
+        <v>595</v>
+      </c>
+      <c r="C45" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" t="s">
+        <v>596</v>
+      </c>
+      <c r="C46" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" t="s">
+        <v>597</v>
+      </c>
+      <c r="C47" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
+        <v>598</v>
+      </c>
+      <c r="C48" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" t="s">
+        <v>599</v>
+      </c>
+      <c r="C49" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" t="s">
+        <v>600</v>
+      </c>
+      <c r="C50" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" t="s">
+        <v>601</v>
+      </c>
+      <c r="C51" t="s">
+        <v>637</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15A0B50-D6E8-4F10-9D30-51785CE2CB65}">
   <dimension ref="A1:A143"/>
   <sheetViews>
@@ -10171,7 +10752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB66B1E-65E4-441B-AD68-3B340E0807A0}">
   <dimension ref="A1:D21"/>
   <sheetViews>

</xml_diff>

<commit_message>
actualizando el esquema de la base de datos
</commit_message>
<xml_diff>
--- a/poblarTorneoFutbol.xlsx
+++ b/poblarTorneoFutbol.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Materias\SSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Materias\SSD\BD_TorneoFutbol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02331ACF-399E-4147-87D9-1AA169E616D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7753F-C7B5-4D6F-AF6D-96ACDDCA3655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nombres" sheetId="1" r:id="rId1"/>
-    <sheet name="Estadio" sheetId="4" r:id="rId2"/>
-    <sheet name="Equipos" sheetId="3" r:id="rId3"/>
-    <sheet name="Dirigentes" sheetId="6" r:id="rId4"/>
-    <sheet name="Apellidos" sheetId="2" r:id="rId5"/>
-    <sheet name="Tecnicos" sheetId="5" r:id="rId6"/>
+    <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
+    <sheet name="Equipos" sheetId="3" r:id="rId2"/>
+    <sheet name="Dirigentes" sheetId="6" r:id="rId3"/>
+    <sheet name="Tecnicos" sheetId="5" r:id="rId4"/>
+    <sheet name="(no colocar)Apellidos" sheetId="2" r:id="rId5"/>
+    <sheet name="(no colocar)Estadios" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2213,7 +2213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2221,13 +2221,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2546,7 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C52DDD2-28BF-4C94-8ED5-EF6546E9B4DB}">
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
       <selection activeCell="B200" sqref="B200:B250"/>
     </sheetView>
   </sheetViews>
@@ -9175,102 +9191,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF9583-190C-41BC-9397-341F69B0C78A}">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>687</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE44EE9-E27F-40A6-848A-C6B51C889E69}">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9279,157 +9204,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>691</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>717</v>
       </c>
     </row>
@@ -9442,11 +9367,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F6090D-08DD-4213-90E6-B42BF7439D3C}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E46" sqref="E46:E47"/>
     </sheetView>
   </sheetViews>
@@ -10022,742 +9947,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15A0B50-D6E8-4F10-9D30-51785CE2CB65}">
-  <dimension ref="A1:A143"/>
-  <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126:A136"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>667</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB66B1E-65E4-441B-AD68-3B340E0807A0}">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11065,4 +10260,825 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15A0B50-D6E8-4F10-9D30-51785CE2CB65}">
+  <dimension ref="A1:A143"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF9583-190C-41BC-9397-341F69B0C78A}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>687</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Poblada de Datos v1
</commit_message>
<xml_diff>
--- a/poblarTorneoFutbol.xlsx
+++ b/poblarTorneoFutbol.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Materias\SSD\BD_TorneoFutbol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7753F-C7B5-4D6F-AF6D-96ACDDCA3655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B775DE72-9901-42B1-BBBB-6A52EA2DACF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="725" activeTab="4" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
     <sheet name="Equipos" sheetId="3" r:id="rId2"/>
-    <sheet name="Dirigentes" sheetId="6" r:id="rId3"/>
-    <sheet name="Tecnicos" sheetId="5" r:id="rId4"/>
-    <sheet name="(no colocar)Apellidos" sheetId="2" r:id="rId5"/>
-    <sheet name="(no colocar)Estadios" sheetId="4" r:id="rId6"/>
+    <sheet name="Clubs" sheetId="8" r:id="rId3"/>
+    <sheet name="Dirigentes" sheetId="6" r:id="rId4"/>
+    <sheet name="Tecnicos" sheetId="5" r:id="rId5"/>
+    <sheet name="(no colocar)Apellidos" sheetId="2" r:id="rId6"/>
+    <sheet name="(no colocar)Estadios" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="786">
   <si>
     <t>Hugo</t>
   </si>
@@ -2114,9 +2115,6 @@
     <t>São Paulo FC (Brazil)</t>
   </si>
   <si>
-    <t>Club América (Mexico)</t>
-  </si>
-  <si>
     <t>Chivas de Guadalajara (Mexico)</t>
   </si>
   <si>
@@ -2126,24 +2124,12 @@
     <t>Tigres UANL (Mexico)</t>
   </si>
   <si>
-    <t>Club Atlético Nacional (Colombia)</t>
-  </si>
-  <si>
     <t>Independiente Santa Fe (Colombia)</t>
   </si>
   <si>
-    <t>Club Olimpia (Paraguay)</t>
-  </si>
-  <si>
     <t>Cerro Porteño (Paraguay)</t>
   </si>
   <si>
-    <t>Club Atlético Peñarol (Uruguay)</t>
-  </si>
-  <si>
-    <t>Club Nacional de Football (Uruguay)</t>
-  </si>
-  <si>
     <t>Colo-Colo (Chile)</t>
   </si>
   <si>
@@ -2162,34 +2148,247 @@
     <t>Barcelona SC (Ecuador)</t>
   </si>
   <si>
-    <t>Club Libertad (Paraguay)</t>
-  </si>
-  <si>
     <t>Deportivo Toluca (Mexico)</t>
   </si>
   <si>
-    <t>Club Atlético Huracán (Argentina)</t>
-  </si>
-  <si>
-    <t>Club Atlético Lanús (Argentina)</t>
-  </si>
-  <si>
-    <t>Club Atlético Vélez Sarsfield (Argentina)</t>
-  </si>
-  <si>
-    <t>Club Deportivo Universidad San Martín (Peru)</t>
-  </si>
-  <si>
-    <t>Club Bolívar (Bolivia)</t>
-  </si>
-  <si>
-    <t>Club The Strongest (Bolivia)</t>
-  </si>
-  <si>
     <t>nombre_equipo</t>
   </si>
   <si>
     <t>id_tipo_tecnico</t>
+  </si>
+  <si>
+    <t>'la mejor'</t>
+  </si>
+  <si>
+    <t>caballo</t>
+  </si>
+  <si>
+    <t>Club The Strongest</t>
+  </si>
+  <si>
+    <t>reloj</t>
+  </si>
+  <si>
+    <t>Club Bolívar</t>
+  </si>
+  <si>
+    <t>celular</t>
+  </si>
+  <si>
+    <t>Club Deportivo Universidad San Martín</t>
+  </si>
+  <si>
+    <t>silla</t>
+  </si>
+  <si>
+    <t>Club Atlético Vélez Sarsfield</t>
+  </si>
+  <si>
+    <t>humamno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club Atlético Lanús </t>
+  </si>
+  <si>
+    <t>raton</t>
+  </si>
+  <si>
+    <t>Club Atlético Huracán</t>
+  </si>
+  <si>
+    <t>tejon</t>
+  </si>
+  <si>
+    <t>club Deportivo Toluca</t>
+  </si>
+  <si>
+    <t>panda</t>
+  </si>
+  <si>
+    <t>club Libertad</t>
+  </si>
+  <si>
+    <t>oso</t>
+  </si>
+  <si>
+    <t>club Barcelona SC</t>
+  </si>
+  <si>
+    <t>fitness</t>
+  </si>
+  <si>
+    <t>club Emelec</t>
+  </si>
+  <si>
+    <t>murcielago</t>
+  </si>
+  <si>
+    <t>club Sporting Cristal</t>
+  </si>
+  <si>
+    <t>espada</t>
+  </si>
+  <si>
+    <t>club Alianza Lima</t>
+  </si>
+  <si>
+    <t>gallina</t>
+  </si>
+  <si>
+    <t>club Universidad de Chile</t>
+  </si>
+  <si>
+    <t>bolivar</t>
+  </si>
+  <si>
+    <t>club Colo-Colo</t>
+  </si>
+  <si>
+    <t>arma</t>
+  </si>
+  <si>
+    <t>club Nacional de Football</t>
+  </si>
+  <si>
+    <t>calavera</t>
+  </si>
+  <si>
+    <t>club Atlético Peñarol</t>
+  </si>
+  <si>
+    <t>rugiente</t>
+  </si>
+  <si>
+    <t>club Cerro Porteño</t>
+  </si>
+  <si>
+    <t>corona</t>
+  </si>
+  <si>
+    <t>club Olimpia</t>
+  </si>
+  <si>
+    <t>aguila</t>
+  </si>
+  <si>
+    <t>club Independiente Santa Fe</t>
+  </si>
+  <si>
+    <t>angel</t>
+  </si>
+  <si>
+    <t>club Atlético Nacional</t>
+  </si>
+  <si>
+    <t>diablo</t>
+  </si>
+  <si>
+    <t>club Tigres UANL</t>
+  </si>
+  <si>
+    <t>pescadito</t>
+  </si>
+  <si>
+    <t>club Cruz Azul</t>
+  </si>
+  <si>
+    <t>moto</t>
+  </si>
+  <si>
+    <t>club Chivas de Guadalajara</t>
+  </si>
+  <si>
+    <t>pelota</t>
+  </si>
+  <si>
+    <t>club América</t>
+  </si>
+  <si>
+    <t>bandera</t>
+  </si>
+  <si>
+    <t>club São Paulo FC</t>
+  </si>
+  <si>
+    <t>escudito</t>
+  </si>
+  <si>
+    <t>club Santos FC</t>
+  </si>
+  <si>
+    <t>loro</t>
+  </si>
+  <si>
+    <t>club Corinthians</t>
+  </si>
+  <si>
+    <t>perro</t>
+  </si>
+  <si>
+    <t>club Flamengo</t>
+  </si>
+  <si>
+    <t>gato</t>
+  </si>
+  <si>
+    <t>club River Plate</t>
+  </si>
+  <si>
+    <t>la mejor'</t>
+  </si>
+  <si>
+    <t>tigre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">club Boca Juniors </t>
+  </si>
+  <si>
+    <t>fecha_creacion</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>Atlético Nacional (Colombia)</t>
+  </si>
+  <si>
+    <t>Olimpia (Paraguay)</t>
+  </si>
+  <si>
+    <t>Atlético Peñarol (Uruguay)</t>
+  </si>
+  <si>
+    <t>Nacional de Football (Uruguay)</t>
+  </si>
+  <si>
+    <t>Atlético Huracán (Argentina)</t>
+  </si>
+  <si>
+    <t>Atlético Lanús (Argentina)</t>
+  </si>
+  <si>
+    <t>Atlético Vélez Sarsfield (Argentina)</t>
+  </si>
+  <si>
+    <t>Deportivo Universidad San Martín (Peru)</t>
+  </si>
+  <si>
+    <t>Bolívar (Bolivia)</t>
+  </si>
+  <si>
+    <t>The Strongest (Bolivia)</t>
+  </si>
+  <si>
+    <t>Libertad (Paraguay)</t>
+  </si>
+  <si>
+    <t>América (Mexico)</t>
+  </si>
+  <si>
+    <t>id_club_futbol</t>
   </si>
 </sst>
 </file>
@@ -2240,11 +2439,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2562,7 +2766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C52DDD2-28BF-4C94-8ED5-EF6546E9B4DB}">
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B200" sqref="B200:B250"/>
     </sheetView>
   </sheetViews>
@@ -9192,170 +9396,264 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE44EE9-E27F-40A6-848A-C6B51C889E69}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>706</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+        <v>777</v>
+      </c>
+      <c r="B26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>778</v>
+      </c>
+      <c r="B27" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>779</v>
+      </c>
+      <c r="B28" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+        <v>780</v>
+      </c>
+      <c r="B29" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+        <v>781</v>
+      </c>
+      <c r="B30" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>717</v>
+        <v>782</v>
+      </c>
+      <c r="B31" s="1">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -9368,11 +9666,465 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC59BB0A-42BC-41F5-9969-202591977C09}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1558</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10983</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D8" s="5">
+        <v>6130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D10" s="5">
+        <v>10004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D11" s="5">
+        <v>21982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D12" s="5">
+        <v>17233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D13" s="5">
+        <v>15035</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D14" s="5">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D15" s="5">
+        <v>4658</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D16" s="5">
+        <v>33509</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D17" s="5">
+        <v>36294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D18" s="5">
+        <v>9241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D19" s="5">
+        <v>7031</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D20" s="5">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D21" s="5">
+        <v>20436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D22" s="5">
+        <v>10711</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D23" s="5">
+        <v>9253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D25" s="5">
+        <v>6253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D26" s="5">
+        <v>5482</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D29" s="5">
+        <v>38007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D30" s="5">
+        <v>9234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D31" s="5">
+        <v>3021</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F6090D-08DD-4213-90E6-B42BF7439D3C}">
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:E47"/>
+      <selection sqref="A1:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9382,563 +10134,563 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>637</v>
       </c>
     </row>
@@ -9947,11 +10699,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB66B1E-65E4-441B-AD68-3B340E0807A0}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -9974,7 +10726,7 @@
         <v>672</v>
       </c>
       <c r="D1" t="s">
-        <v>719</v>
+        <v>707</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10262,7 +11014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15A0B50-D6E8-4F10-9D30-51785CE2CB65}">
   <dimension ref="A1:A143"/>
   <sheetViews>
@@ -10992,7 +11744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF9583-190C-41BC-9397-341F69B0C78A}">
   <dimension ref="A1:A15"/>
   <sheetViews>

</xml_diff>

<commit_message>
Poblada de Datos v2
</commit_message>
<xml_diff>
--- a/poblarTorneoFutbol.xlsx
+++ b/poblarTorneoFutbol.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Materias\SSD\BD_TorneoFutbol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B775DE72-9901-42B1-BBBB-6A52EA2DACF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97259D50-AC1C-4C9C-97C7-90CBA067C781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="725" activeTab="4" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="725" xr2:uid="{732F3510-D69B-4D80-8B51-8013CF9E5EAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
-    <sheet name="Equipos" sheetId="3" r:id="rId2"/>
+    <sheet name="Dirigentes" sheetId="6" r:id="rId2"/>
     <sheet name="Clubs" sheetId="8" r:id="rId3"/>
-    <sheet name="Dirigentes" sheetId="6" r:id="rId4"/>
-    <sheet name="Tecnicos" sheetId="5" r:id="rId5"/>
+    <sheet name="Tecnicos" sheetId="5" r:id="rId4"/>
+    <sheet name="Equipos" sheetId="3" r:id="rId5"/>
     <sheet name="(no colocar)Apellidos" sheetId="2" r:id="rId6"/>
     <sheet name="(no colocar)Estadios" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -2766,7 +2766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C52DDD2-28BF-4C94-8ED5-EF6546E9B4DB}">
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B200" sqref="B200:B250"/>
     </sheetView>
   </sheetViews>
@@ -9395,273 +9395,582 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE44EE9-E27F-40A6-848A-C6B51C889E69}">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F6090D-08DD-4213-90E6-B42BF7439D3C}">
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>706</v>
+        <v>670</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>690</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>695</v>
-      </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="B14" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="B16" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="B17" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="B18" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="B19" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B20" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="B21" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="B22" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="B23" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="B24" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>705</v>
-      </c>
-      <c r="B25" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="B26" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="B27" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>779</v>
-      </c>
-      <c r="B28" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>780</v>
-      </c>
-      <c r="B29" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="B30" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="B31" s="1">
-        <v>30</v>
+        <v>82</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>637</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A74">
-    <sortCondition ref="A2:A74"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10120,590 +10429,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F6090D-08DD-4213-90E6-B42BF7439D3C}">
-  <dimension ref="A1:C51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>637</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB66B1E-65E4-441B-AD68-3B340E0807A0}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -11011,6 +10740,277 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE44EE9-E27F-40A6-848A-C6B51C889E69}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="B25" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="B27" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B28" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="B29" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B30" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B31" s="1">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A74">
+    <sortCondition ref="A2:A74"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>